<commit_message>
modification task et codesystem
ajout demandé par ROR et traitement du warning caseSensitive sur les codeSystems da519ca534f29228e974717e3e8159324d527493
</commit_message>
<xml_diff>
--- a/ig/anomalies/CodeSystem-input-task-ror-codesystem.xlsx
+++ b/ig/anomalies/CodeSystem-input-task-ror-codesystem.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-11T09:40:11+00:00</t>
+    <t>2023-04-12T13:10:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Case Sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Value Set (all codes)</t>
@@ -406,54 +409,56 @@
       <c r="A14" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -471,100 +476,100 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>